<commit_message>
Add Data/ Fix Calibration
</commit_message>
<xml_diff>
--- a/DATA/IDS_SRI+PAK_WORLD+CHINA.xlsx
+++ b/DATA/IDS_SRI+PAK_WORLD+CHINA.xlsx
@@ -278,12 +278,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="0.000E+00"/>
     <numFmt numFmtId="60" formatCode="0.00&quot; &quot;;(0.00)"/>
     <numFmt numFmtId="61" formatCode="0.0000%"/>
-    <numFmt numFmtId="62" formatCode="0.00_);\(0.00\)"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -326,7 +325,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -347,35 +346,35 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -392,7 +391,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -400,14 +399,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -417,26 +416,23 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -466,10 +462,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -484,7 +477,7 @@
     <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="61" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="61" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -521,10 +514,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="fffde9d9"/>
-      <rgbColor rgb="ffd8d8d8"/>
+      <rgbColor rgb="ffd9d9d9"/>
       <rgbColor rgb="ff595959"/>
       <rgbColor rgb="ffff0000"/>
     </indexedColors>
@@ -567,10 +560,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.371313"/>
+          <c:x val="0.385267"/>
           <c:y val="0"/>
-          <c:w val="0.257374"/>
-          <c:h val="0.132417"/>
+          <c:w val="0.251971"/>
+          <c:h val="0.134093"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -586,10 +579,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.113817"/>
-          <c:y val="0.132417"/>
-          <c:w val="0.881183"/>
-          <c:h val="0.696709"/>
+          <c:x val="0.133932"/>
+          <c:y val="0.134093"/>
+          <c:w val="0.861068"/>
+          <c:h val="0.693028"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -622,7 +615,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
-            <c:size val="4"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000">
@@ -775,7 +768,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
-            <c:size val="4"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000">
@@ -928,7 +921,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
-            <c:size val="4"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000">
@@ -1081,7 +1074,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
-            <c:size val="4"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000">
@@ -1315,10 +1308,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.00261471"/>
-          <c:y val="0.93761"/>
-          <c:w val="0.906947"/>
-          <c:h val="0.06239"/>
+          <c:x val="0"/>
+          <c:y val="0.936978"/>
+          <c:w val="0.938036"/>
+          <c:h val="0.0630216"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1399,10 +1392,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.376054"/>
+          <c:x val="0.375826"/>
           <c:y val="0"/>
-          <c:w val="0.247892"/>
-          <c:h val="0.132417"/>
+          <c:w val="0.248348"/>
+          <c:h val="0.134093"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1418,10 +1411,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.109225"/>
-          <c:y val="0.132417"/>
-          <c:w val="0.885775"/>
-          <c:h val="0.696709"/>
+          <c:x val="0.109425"/>
+          <c:y val="0.134093"/>
+          <c:w val="0.885575"/>
+          <c:h val="0.693028"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1454,7 +1447,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
-            <c:size val="4"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000">
@@ -1607,7 +1600,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
-            <c:size val="4"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000">
@@ -1760,7 +1753,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
-            <c:size val="4"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000">
@@ -1913,7 +1906,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
-            <c:size val="4"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000">
@@ -2050,7 +2043,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0.00_);\(0.00\)" sourceLinked="0"/>
+        <c:numFmt formatCode="0.00&quot; &quot;;(0.00)" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -2147,10 +2140,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0978785"/>
-          <c:y val="0.93761"/>
-          <c:w val="0.83077"/>
-          <c:h val="0.06239"/>
+          <c:x val="0.0745635"/>
+          <c:y val="0.936978"/>
+          <c:w val="0.879286"/>
+          <c:h val="0.0630216"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2201,15 +2194,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>447721</xdr:colOff>
+      <xdr:colOff>333691</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>16207</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>23494</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>24726</xdr:rowOff>
+      <xdr:colOff>15836</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>186544</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2217,8 +2210,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9998121" y="397207"/>
-        <a:ext cx="4960574" cy="2294520"/>
+        <a:off x="9884091" y="397207"/>
+        <a:ext cx="5066946" cy="2265838"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2242,9 +2235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>42544</xdr:colOff>
+      <xdr:colOff>32611</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>39966</xdr:rowOff>
+      <xdr:rowOff>11284</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2253,7 +2246,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6984218" y="221947"/>
-        <a:ext cx="5415427" cy="2294520"/>
+        <a:ext cx="5405494" cy="2265838"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2411,9 +2404,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -2493,7 +2486,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2521,10 +2514,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2780,9 +2773,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -3070,7 +3063,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3098,10 +3091,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -4398,818 +4391,818 @@
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" t="s" s="6">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="6">
+      <c r="B1" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="C1" t="s" s="6">
+      <c r="C1" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="D1" t="s" s="6">
+      <c r="D1" t="s" s="2">
         <v>58</v>
       </c>
-      <c r="E1" t="s" s="6">
+      <c r="E1" t="s" s="2">
         <v>58</v>
       </c>
     </row>
     <row r="2" ht="16" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="E2" t="s" s="6">
+      <c r="E2" t="s" s="2">
         <v>59</v>
       </c>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="A3" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" t="s" s="2">
         <v>56</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="E3" t="s" s="2">
         <v>56</v>
       </c>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="A4" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="6">
+      <c r="B4" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="C4" t="s" s="6">
+      <c r="C4" t="s" s="2">
         <v>57</v>
       </c>
-      <c r="D4" t="s" s="6">
+      <c r="D4" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="E4" t="s" s="6">
+      <c r="E4" t="s" s="2">
         <v>57</v>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" t="s" s="6">
+      <c r="A5" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="B5" t="s" s="6">
+      <c r="B5" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="C5" t="s" s="6">
+      <c r="C5" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="D5" t="s" s="6">
+      <c r="D5" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="E5" t="s" s="6">
+      <c r="E5" t="s" s="2">
         <v>54</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="A6" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>1849029664.4</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>29061718.5</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>9931198662.299999</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>149430945.3</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" t="s" s="6">
+      <c r="A7" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>2241837854.3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>38197055.1</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>10580767699.9</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>142538092.9</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" t="s" s="6">
+      <c r="A8" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>2632029310.2</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>37828578.5</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>11703994182.1</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>183526646.8</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" t="s" s="6">
+      <c r="A9" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>2890238573.3</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>34879303.7</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>12026223274.4</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>180689717.9</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" t="s" s="6">
+      <c r="A10" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>2998355044.3</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>24764306.3</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>12227885011.6</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>143266648.8</v>
       </c>
     </row>
     <row r="11" ht="16" customHeight="1">
-      <c r="A11" t="s" s="6">
+      <c r="A11" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>3544639145.8</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>22660368.2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>13464882307</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>151726191.1</v>
       </c>
     </row>
     <row r="12" ht="16" customHeight="1">
-      <c r="A12" t="s" s="6">
+      <c r="A12" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>4086689689.8</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>33344902.4</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>14954407650.6</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>148616183.2</v>
       </c>
     </row>
     <row r="13" ht="16" customHeight="1">
-      <c r="A13" t="s" s="6">
+      <c r="A13" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>4754428931.3</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>40316675.9</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>16797670141.1</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>144943981.1</v>
       </c>
     </row>
     <row r="14" ht="16" customHeight="1">
-      <c r="A14" t="s" s="6">
+      <c r="A14" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>5209633062.8</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>42911979.9</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>17065165352.3</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>141221659.6</v>
       </c>
     </row>
     <row r="15" ht="16" customHeight="1">
-      <c r="A15" t="s" s="6">
+      <c r="A15" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>5185722277.5</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>35812212.9</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>18348188708.1</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>179186617.6</v>
       </c>
     </row>
     <row r="16" ht="16" customHeight="1">
-      <c r="A16" t="s" s="6">
+      <c r="A16" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>5867509111.8</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>23453394</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>20663375831.9</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>228017067.9</v>
       </c>
     </row>
     <row r="17" ht="16" customHeight="1">
-      <c r="A17" t="s" s="6">
+      <c r="A17" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>6580740209.6</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>23053251.9</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>23363317172.7</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>243972711.4</v>
       </c>
     </row>
     <row r="18" ht="16" customHeight="1">
-      <c r="A18" t="s" s="6">
+      <c r="A18" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>6476089777.8</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>20229838.7</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>24919617589.9</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>281658096.9</v>
       </c>
     </row>
     <row r="19" ht="16" customHeight="1">
-      <c r="A19" t="s" s="6">
+      <c r="A19" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>6902629411</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>18454827.9</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>24551561529.1</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>373839795</v>
       </c>
     </row>
     <row r="20" ht="16" customHeight="1">
-      <c r="A20" t="s" s="6">
+      <c r="A20" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>7960615109.6</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>11569459.5</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>27390827116.9</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>432545708.6</v>
       </c>
     </row>
     <row r="21" ht="16" customHeight="1">
-      <c r="A21" t="s" s="6">
+      <c r="A21" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>8395502196.9</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>13270134.8</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>30241086482.6</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>417158836.8</v>
       </c>
     </row>
     <row r="22" ht="16" customHeight="1">
-      <c r="A22" t="s" s="6">
+      <c r="A22" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>8298763054.9</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>12151072.4</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>29850953918.3</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>439801891</v>
       </c>
     </row>
     <row r="23" ht="16" customHeight="1">
-      <c r="A23" t="s" s="6">
+      <c r="A23" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>8106316372.4</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>14002757.9</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>30095124742.1</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>599300423.8</v>
       </c>
     </row>
     <row r="24" ht="16" customHeight="1">
-      <c r="A24" t="s" s="6">
+      <c r="A24" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>9057333356.1</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>24686360.9</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>32310194703.8</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>589065227.1</v>
       </c>
     </row>
     <row r="25" ht="16" customHeight="1">
-      <c r="A25" t="s" s="6">
+      <c r="A25" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>9943050525</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>27584265.2</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>34192272492.3</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>603140475.6</v>
       </c>
     </row>
     <row r="26" ht="16" customHeight="1">
-      <c r="A26" t="s" s="6">
+      <c r="A26" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>9249848286.4</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>27190546.8</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>33111988980.4</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>653213444.8</v>
       </c>
     </row>
     <row r="27" ht="16" customHeight="1">
-      <c r="A27" t="s" s="6">
+      <c r="A27" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>8952124828.1</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>39324219.2</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>32046178980.2</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>94910472.7</v>
       </c>
     </row>
     <row r="28" ht="16" customHeight="1">
-      <c r="A28" t="s" s="6">
+      <c r="A28" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>10122942033.8</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>70084282.59999999</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>33967034723.9</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>137947155.1</v>
       </c>
     </row>
     <row r="29" ht="16" customHeight="1">
-      <c r="A29" t="s" s="6">
+      <c r="A29" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>10725993550</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>88122246.3</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>36668571730.4</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>340927338.7</v>
       </c>
     </row>
     <row r="30" ht="16" customHeight="1">
-      <c r="A30" t="s" s="6">
+      <c r="A30" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>11600420988.8</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>99449151.59999999</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>36561942040.2</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>523590010.8</v>
       </c>
     </row>
     <row r="31" ht="16" customHeight="1">
-      <c r="A31" t="s" s="6">
+      <c r="A31" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>11300134209.5</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>99698796.09999999</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>34260045290.9</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>610510191.2</v>
       </c>
     </row>
     <row r="32" ht="16" customHeight="1">
-      <c r="A32" t="s" s="8">
+      <c r="A32" t="s" s="7">
         <v>32</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="8">
         <v>11853449200.4</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>103154256.6</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="8">
         <v>37430775913.1</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <v>981308438.1</v>
       </c>
     </row>
     <row r="33" ht="16" customHeight="1">
-      <c r="A33" t="s" s="10">
+      <c r="A33" t="s" s="9">
         <v>33</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="10">
         <v>14161321567.6</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="10">
         <v>271623707.3</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="10">
         <v>42306089047.4</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="11">
         <v>1103942201.5</v>
       </c>
     </row>
     <row r="34" ht="16" customHeight="1">
-      <c r="A34" t="s" s="10">
+      <c r="A34" t="s" s="9">
         <v>34</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="10">
         <v>16320821885.1</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="10">
         <v>313267189.9</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="10">
         <v>49826301249</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="11">
         <v>1131082172</v>
       </c>
     </row>
     <row r="35" ht="16" customHeight="1">
-      <c r="A35" t="s" s="10">
+      <c r="A35" t="s" s="9">
         <v>35</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B35" s="10">
         <v>19504201128</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="10">
         <v>602965075.2</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="10">
         <v>56662922386.2</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="11">
         <v>2008517395.2</v>
       </c>
     </row>
     <row r="36" ht="16" customHeight="1">
-      <c r="A36" t="s" s="10">
+      <c r="A36" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B36" s="11">
+      <c r="B36" s="10">
         <v>21684210688.5</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="10">
         <v>1443092440.3</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="10">
         <v>63124246853.5</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="11">
         <v>2182715088.4</v>
       </c>
     </row>
     <row r="37" ht="16" customHeight="1">
-      <c r="A37" t="s" s="10">
+      <c r="A37" t="s" s="9">
         <v>37</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B37" s="10">
         <v>25795379781.1</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="10">
         <v>1875694551.9</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="10">
         <v>64742561800.2</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="11">
         <v>2623586522.7</v>
       </c>
     </row>
     <row r="38" ht="16" customHeight="1">
-      <c r="A38" t="s" s="10">
+      <c r="A38" t="s" s="9">
         <v>38</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B38" s="10">
         <v>35735908567.5</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="10">
         <v>2716626375.7</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="10">
         <v>63669520213.6</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E38" s="11">
         <v>3310938888</v>
       </c>
     </row>
     <row r="39" ht="16" customHeight="1">
-      <c r="A39" t="s" s="10">
+      <c r="A39" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="10">
         <v>39314598514.4</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="10">
         <v>3633004552.6</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="10">
         <v>60087820820.5</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="11">
         <v>4229593003.8</v>
       </c>
     </row>
     <row r="40" ht="16" customHeight="1">
-      <c r="A40" t="s" s="10">
+      <c r="A40" t="s" s="9">
         <v>40</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="10">
         <v>42262761571.6</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="10">
         <v>4307694238.5</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="10">
         <v>64202720545.2</v>
       </c>
-      <c r="E40" s="12">
+      <c r="E40" s="11">
         <v>5138871586.5</v>
       </c>
     </row>
     <row r="41" ht="16" customHeight="1">
-      <c r="A41" t="s" s="10">
+      <c r="A41" t="s" s="9">
         <v>41</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="10">
         <v>43925393891.1</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="10">
         <v>4523983040.5</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="10">
         <v>68614186760.2</v>
       </c>
-      <c r="E41" s="12">
+      <c r="E41" s="11">
         <v>5988725755.7</v>
       </c>
     </row>
     <row r="42" ht="16" customHeight="1">
-      <c r="A42" t="s" s="10">
+      <c r="A42" t="s" s="9">
         <v>42</v>
       </c>
-      <c r="B42" s="11">
+      <c r="B42" s="10">
         <v>46661458616.2</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="10">
         <v>4679819369.1</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D42" s="10">
         <v>75052145049.5</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="11">
         <v>7636999126.9</v>
       </c>
     </row>
     <row r="43" ht="16" customHeight="1">
-      <c r="A43" t="s" s="10">
+      <c r="A43" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="B43" s="11">
+      <c r="B43" s="10">
         <v>50765545978.7</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="10">
         <v>5081537216.7</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D43" s="10">
         <v>91662069234.5</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E43" s="11">
         <v>10996185969.5</v>
       </c>
     </row>
     <row r="44" ht="16" customHeight="1">
-      <c r="A44" t="s" s="13">
+      <c r="A44" t="s" s="12">
         <v>44</v>
       </c>
-      <c r="B44" s="14">
+      <c r="B44" s="13">
         <v>52919692662.2</v>
       </c>
-      <c r="C44" s="14">
+      <c r="C44" s="13">
         <v>6067017951.6</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="13">
         <v>99223959504.7</v>
       </c>
-      <c r="E44" s="14">
+      <c r="E44" s="13">
         <v>18131675381</v>
       </c>
     </row>
     <row r="45" ht="16" customHeight="1">
-      <c r="A45" t="s" s="6">
+      <c r="A45" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="6">
         <v>56117855647</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="6">
         <v>6382384375.8</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <v>107882935628.6</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="6">
         <v>21619974718</v>
       </c>
     </row>
     <row r="46" ht="16" customHeight="1">
-      <c r="A46" t="s" s="6">
+      <c r="A46" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="6">
         <v>56299454219.9</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="6">
         <v>6832918923.4</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="6">
         <v>115695344143.7</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="6">
         <v>22982050873.2</v>
       </c>
     </row>
     <row r="47" ht="16" customHeight="1">
-      <c r="A47" t="s" s="6">
+      <c r="A47" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="6">
         <v>56592086411.4</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <v>7215683975.8</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <v>130433056375.4</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="6">
         <v>27358303315.7</v>
       </c>
     </row>
     <row r="48" ht="16" customHeight="1">
-      <c r="A48" t="s" s="6">
+      <c r="A48" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="B48" t="s" s="6">
+      <c r="B48" t="s" s="2">
         <v>55</v>
       </c>
-      <c r="C48" t="s" s="6">
+      <c r="C48" t="s" s="2">
         <v>55</v>
       </c>
-      <c r="D48" t="s" s="6">
+      <c r="D48" t="s" s="2">
         <v>55</v>
       </c>
-      <c r="E48" t="s" s="6">
+      <c r="E48" t="s" s="2">
         <v>55</v>
       </c>
     </row>
@@ -5230,20 +5223,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.1719" style="15" customWidth="1"/>
-    <col min="2" max="2" width="16" style="15" customWidth="1"/>
-    <col min="3" max="3" width="23.6719" style="15" customWidth="1"/>
-    <col min="4" max="4" width="19.8516" style="15" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="15" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="15" customWidth="1"/>
+    <col min="1" max="1" width="15.1719" style="14" customWidth="1"/>
+    <col min="2" max="2" width="16" style="14" customWidth="1"/>
+    <col min="3" max="3" width="23.6719" style="14" customWidth="1"/>
+    <col min="4" max="4" width="19.8516" style="14" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
       <c r="A1" s="4"/>
-      <c r="B1" t="s" s="6">
+      <c r="B1" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="C1" t="s" s="6">
+      <c r="C1" t="s" s="2">
         <v>58</v>
       </c>
       <c r="D1" t="s" s="2">
@@ -5257,12 +5250,12 @@
       <c r="A2" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="15">
         <v>5024000000</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="15">
         <v>30938000000</v>
       </c>
     </row>
@@ -5270,12 +5263,12 @@
       <c r="A3" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15">
         <v>5228000000</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="15">
         <v>36599000000</v>
       </c>
     </row>
@@ -5283,12 +5276,12 @@
       <c r="A4" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="15">
         <v>5644000000</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="15">
         <v>40012000000</v>
       </c>
     </row>
@@ -5296,12 +5289,12 @@
       <c r="A5" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="15">
         <v>6093000000</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="15">
         <v>37369000000</v>
       </c>
     </row>
@@ -5309,12 +5302,12 @@
       <c r="A6" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="15">
         <v>7142000000</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="15">
         <v>40572000000</v>
       </c>
     </row>
@@ -5322,12 +5315,12 @@
       <c r="A7" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="15">
         <v>7064000000</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="15">
         <v>40565000000</v>
       </c>
     </row>
@@ -5335,12 +5328,12 @@
       <c r="A8" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="15">
         <v>7571000000</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="15">
         <v>41543000000</v>
       </c>
     </row>
@@ -5348,12 +5341,12 @@
       <c r="A9" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="15">
         <v>7884000000</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="15">
         <v>43437000000</v>
       </c>
     </row>
@@ -5361,12 +5354,12 @@
       <c r="A10" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="15">
         <v>8240000000</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="15">
         <v>50107000000</v>
       </c>
     </row>
@@ -5374,12 +5367,12 @@
       <c r="A11" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="15">
         <v>8271000000</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="15">
         <v>52256000000</v>
       </c>
     </row>
@@ -5387,12 +5380,12 @@
       <c r="A12" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="15">
         <v>9468000000</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="15">
         <v>52426000000</v>
       </c>
     </row>
@@ -5400,12 +5393,12 @@
       <c r="A13" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="15">
         <v>10367000000</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="15">
         <v>59556000000</v>
       </c>
     </row>
@@ -5413,12 +5406,12 @@
       <c r="A14" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="15">
         <v>11176000000</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="15">
         <v>63727000000</v>
       </c>
     </row>
@@ -5426,12 +5419,12 @@
       <c r="A15" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="15">
         <v>11948000000</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="15">
         <v>67442000000</v>
       </c>
     </row>
@@ -5439,12 +5432,12 @@
       <c r="A16" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="15">
         <v>13781000000</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="15">
         <v>67998000000</v>
       </c>
     </row>
@@ -5452,12 +5445,12 @@
       <c r="A17" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="15">
         <v>14635000000</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="15">
         <v>79451000000</v>
       </c>
     </row>
@@ -5465,12 +5458,12 @@
       <c r="A18" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="15">
         <v>16051000000</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="15">
         <v>82968000000</v>
       </c>
     </row>
@@ -5478,12 +5471,12 @@
       <c r="A19" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="17">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="15">
         <v>17888000000</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="15">
         <v>81806000000</v>
       </c>
     </row>
@@ -5491,12 +5484,12 @@
       <c r="A20" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="15">
         <v>18430000000</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="15">
         <v>81490000000</v>
       </c>
     </row>
@@ -5504,12 +5497,12 @@
       <c r="A21" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="17">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="15">
         <v>18532000000</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="15">
         <v>82514000000</v>
       </c>
     </row>
@@ -5517,16 +5510,16 @@
       <c r="A22" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="16">
         <v>0</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="16">
         <v>2374003.75</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="15">
         <v>19371000000</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="15">
         <v>79705000000</v>
       </c>
     </row>
@@ -5534,16 +5527,16 @@
       <c r="A23" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="16">
         <v>0</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="16">
         <v>789556625.875</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="15">
         <v>18610000000</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="15">
         <v>77931000000</v>
       </c>
     </row>
@@ -5551,16 +5544,16 @@
       <c r="A24" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="16">
         <v>0</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="16">
         <v>808461700.5</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="15">
         <v>19585000000</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="15">
         <v>77937000000</v>
       </c>
     </row>
@@ -5568,16 +5561,16 @@
       <c r="A25" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="16">
         <v>6300000</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="16">
         <v>1268858265.875</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="15">
         <v>21621000000</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="15">
         <v>89727000000</v>
       </c>
     </row>
@@ -5585,16 +5578,16 @@
       <c r="A26" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="16">
         <v>6300000</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="16">
         <v>1268825885.5</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="15">
         <v>23655000000</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="15">
         <v>105612000000</v>
       </c>
     </row>
@@ -5602,16 +5595,16 @@
       <c r="A27" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="16">
         <v>313300000</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="16">
         <v>1315456168.375</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="15">
         <v>27945000000</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="15">
         <v>118481000000</v>
       </c>
     </row>
@@ -5619,16 +5612,16 @@
       <c r="A28" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="16">
         <v>943300000</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="16">
         <v>1774863503.125</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="15">
         <v>32359000000</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="15">
         <v>137229000000</v>
       </c>
     </row>
@@ -5636,16 +5629,16 @@
       <c r="A29" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="16">
         <v>943300000</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="16">
         <v>1695388803.25</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="15">
         <v>37043000000</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="15">
         <v>152362000000</v>
       </c>
     </row>
@@ -5653,16 +5646,16 @@
       <c r="A30" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="16">
         <v>982000000</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="16">
         <v>2647238076.125</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="15">
         <v>46602000000</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="15">
         <v>170853000000</v>
       </c>
     </row>
@@ -5670,16 +5663,16 @@
       <c r="A31" t="s" s="2">
         <v>35</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="16">
         <v>3230274192</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="16">
         <v>3372958745.75</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="15">
         <v>48113000000</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="15">
         <v>167875000000</v>
       </c>
     </row>
@@ -5687,16 +5680,16 @@
       <c r="A32" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="B32" s="18">
+      <c r="B32" s="16">
         <v>4020008096</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="16">
         <v>5205926015.6875</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="15">
         <v>56710000000</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="15">
         <v>177166000000</v>
       </c>
     </row>
@@ -5704,16 +5697,16 @@
       <c r="A33" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="B33" s="18">
+      <c r="B33" s="16">
         <v>4785999130</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="16">
         <v>5098878486.375</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="15">
         <v>65267000000</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="15">
         <v>213588000000</v>
       </c>
     </row>
@@ -5721,16 +5714,16 @@
       <c r="A34" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="16">
         <v>5065012462</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="16">
         <v>4951854278.25</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="15">
         <v>68419000000</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="15">
         <v>224384000000</v>
       </c>
     </row>
@@ -5738,16 +5731,16 @@
       <c r="A35" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="16">
         <v>5477187102</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="16">
         <v>4795856077.1875</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="15">
         <v>74277000000</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="15">
         <v>231218000000</v>
       </c>
     </row>
@@ -5755,16 +5748,16 @@
       <c r="A36" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="B36" s="18">
+      <c r="B36" s="16">
         <v>7547451226</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="16">
         <v>12949317715.125</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="15">
         <v>79312000000</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="15">
         <v>244361000000</v>
       </c>
     </row>
@@ -5772,16 +5765,16 @@
       <c r="A37" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="16">
         <v>7219605762</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="16">
         <v>15294148136.5</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="15">
         <v>80412000000</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="15">
         <v>270556000000</v>
       </c>
     </row>
@@ -5789,16 +5782,16 @@
       <c r="A38" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38" s="16">
         <v>7216834010</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="16">
         <v>24895138153.4688</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="15">
         <v>81546000000</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="15">
         <v>278655000000</v>
       </c>
     </row>
@@ -5806,16 +5799,16 @@
       <c r="A39" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="B39" s="18">
+      <c r="B39" s="16">
         <v>7305812611</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="16">
         <v>27632803070.6875</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="15">
         <v>87348000000</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="15">
         <v>304952000000</v>
       </c>
     </row>
@@ -5823,8 +5816,8 @@
       <c r="A40" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
@@ -5832,8 +5825,8 @@
       <c r="A41" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
@@ -5841,8 +5834,8 @@
       <c r="A42" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
     </row>
@@ -5850,8 +5843,8 @@
       <c r="A43" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
     </row>
@@ -5859,29 +5852,29 @@
       <c r="A44" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
     </row>
     <row r="45" ht="16" customHeight="1">
       <c r="A45" s="4"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
     </row>
     <row r="46" ht="16" customHeight="1">
       <c r="A46" s="4"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
     </row>
     <row r="47" ht="16" customHeight="1">
       <c r="A47" s="4"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
     </row>
@@ -5889,10 +5882,10 @@
       <c r="A48" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="B48" t="s" s="6">
+      <c r="B48" t="s" s="2">
         <v>65</v>
       </c>
-      <c r="C48" s="16"/>
+      <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
     </row>
@@ -5913,26 +5906,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="27.6719" style="19" customWidth="1"/>
-    <col min="3" max="3" width="14.6719" style="19" customWidth="1"/>
-    <col min="4" max="4" width="27.6719" style="19" customWidth="1"/>
-    <col min="5" max="5" width="18.8516" style="19" customWidth="1"/>
-    <col min="6" max="15" width="8.85156" style="19" customWidth="1"/>
-    <col min="16" max="16384" width="8.85156" style="19" customWidth="1"/>
+    <col min="1" max="2" width="27.6719" style="17" customWidth="1"/>
+    <col min="3" max="3" width="14.6719" style="17" customWidth="1"/>
+    <col min="4" max="4" width="27.6719" style="17" customWidth="1"/>
+    <col min="5" max="5" width="18.8516" style="17" customWidth="1"/>
+    <col min="6" max="15" width="8.85156" style="17" customWidth="1"/>
+    <col min="16" max="16384" width="8.85156" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" s="4"/>
-      <c r="B1" t="s" s="6">
+      <c r="B1" t="s" s="2">
         <v>66</v>
       </c>
-      <c r="C1" t="s" s="6">
+      <c r="C1" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="D1" t="s" s="6">
+      <c r="D1" t="s" s="2">
         <v>67</v>
       </c>
-      <c r="E1" t="s" s="6">
+      <c r="E1" t="s" s="2">
         <v>58</v>
       </c>
       <c r="F1" s="4"/>
@@ -5950,19 +5943,19 @@
       <c r="A2" s="3">
         <v>2007</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="16">
         <f>'Transposed'!B33-'Transposed'!C33</f>
         <v>13889697860.3</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="16">
         <f>B2+'China Debt Data'!B29</f>
         <v>14832997860.3</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="16">
         <f>'Transposed'!D33-'Transposed'!E33</f>
         <v>41202146845.9</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="16">
         <f>D2+'China Debt Data'!C29</f>
         <v>42897535649.15</v>
       </c>
@@ -5981,19 +5974,19 @@
       <c r="A3" s="3">
         <v>2008</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <f>'Transposed'!B34-'Transposed'!C34</f>
         <v>16007554695.2</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="16">
         <f>B3+'China Debt Data'!B30</f>
         <v>16989554695.2</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="16">
         <f>'Transposed'!D34-'Transposed'!E34</f>
         <v>48695219077</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="16">
         <f>D3+'China Debt Data'!C30</f>
         <v>51342457153.125</v>
       </c>
@@ -6012,19 +6005,19 @@
       <c r="A4" s="3">
         <v>2009</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <f>'Transposed'!B35-'Transposed'!C35</f>
         <v>18901236052.8</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <f>B4+'China Debt Data'!B31</f>
         <v>22131510244.8</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <f>'Transposed'!D35-'Transposed'!E35</f>
         <v>54654404991</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="16">
         <f>D4+'China Debt Data'!C31</f>
         <v>58027363736.75</v>
       </c>
@@ -6043,19 +6036,19 @@
       <c r="A5" s="3">
         <v>2010</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <f>'Transposed'!B36-'Transposed'!C36</f>
         <v>20241118248.2</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <f>B5+'China Debt Data'!B32</f>
         <v>24261126344.2</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <f>'Transposed'!D36-'Transposed'!E36</f>
         <v>60941531765.1</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="16">
         <f>D5+'China Debt Data'!C32</f>
         <v>66147457780.7875</v>
       </c>
@@ -6074,19 +6067,19 @@
       <c r="A6" s="3">
         <v>2011</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <f>'Transposed'!B37-'Transposed'!C37</f>
         <v>23919685229.2</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <f>B6+'China Debt Data'!B33</f>
         <v>28705684359.2</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <f>'Transposed'!D37-'Transposed'!E37</f>
         <v>62118975277.5</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <f>D6+'China Debt Data'!C33</f>
         <v>67217853763.875</v>
       </c>
@@ -6105,19 +6098,19 @@
       <c r="A7" s="3">
         <v>2012</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <f>'Transposed'!B38-'Transposed'!C38</f>
         <v>33019282191.8</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <f>B7+'China Debt Data'!B34</f>
         <v>38084294653.8</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <f>'Transposed'!D38-'Transposed'!E38</f>
         <v>60358581325.6</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <f>D7+'China Debt Data'!C34</f>
         <v>65310435603.85</v>
       </c>
@@ -6136,19 +6129,19 @@
       <c r="A8" s="3">
         <v>2013</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <f>'Transposed'!B39-'Transposed'!C39</f>
         <v>35681593961.8</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <f>B8+'China Debt Data'!B35</f>
         <v>41158781063.8</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <f>'Transposed'!D39-'Transposed'!E39</f>
         <v>55858227816.7</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <f>D8+'China Debt Data'!C35</f>
         <v>60654083893.8875</v>
       </c>
@@ -6167,19 +6160,19 @@
       <c r="A9" s="3">
         <v>2014</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="16">
         <f>'Transposed'!B40-'Transposed'!C40</f>
         <v>37955067333.1</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="16">
         <f>B9+'China Debt Data'!B36</f>
         <v>45502518559.1</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <f>'Transposed'!D40-'Transposed'!E40</f>
         <v>59063848958.7</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="16">
         <f>D9+'China Debt Data'!C36</f>
         <v>72013166673.825</v>
       </c>
@@ -6198,19 +6191,19 @@
       <c r="A10" s="3">
         <v>2015</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="16">
         <f>'Transposed'!B41-'Transposed'!C41</f>
         <v>39401410850.6</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="16">
         <f>B10+'China Debt Data'!B37</f>
         <v>46621016612.6</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <f>'Transposed'!D41-'Transposed'!E41</f>
         <v>62625461004.5</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <f>D10+'China Debt Data'!C37</f>
         <v>77919609141</v>
       </c>
@@ -6229,19 +6222,19 @@
       <c r="A11" s="3">
         <v>2016</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="16">
         <f>'Transposed'!B42-'Transposed'!C42</f>
         <v>41981639247.1</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="16">
         <f>B11+'China Debt Data'!B38</f>
         <v>49198473257.1</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <f>'Transposed'!D42-'Transposed'!E42</f>
         <v>67415145922.6</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="16">
         <f>D11+'China Debt Data'!C38</f>
         <v>92310284076.0688</v>
       </c>
@@ -6260,19 +6253,19 @@
       <c r="A12" s="3">
         <v>2017</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="16">
         <f>'Transposed'!B43-'Transposed'!C43</f>
         <v>45684008762</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="16">
         <f>B12+'China Debt Data'!B39</f>
         <v>52989821373</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <f>'Transposed'!D43-'Transposed'!E43</f>
         <v>80665883265</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="16">
         <f>D12+'China Debt Data'!C39</f>
         <v>108298686335.688</v>
       </c>
@@ -6289,10 +6282,10 @@
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="4"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -6306,10 +6299,10 @@
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" s="4"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -6323,10 +6316,10 @@
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -6340,10 +6333,10 @@
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" s="4"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -6373,17 +6366,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="20" customWidth="1"/>
-    <col min="2" max="2" width="23.3516" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.85156" style="20" customWidth="1"/>
-    <col min="4" max="4" width="22" style="20" customWidth="1"/>
-    <col min="5" max="5" width="9.85156" style="20" customWidth="1"/>
-    <col min="6" max="16" width="8.85156" style="20" customWidth="1"/>
-    <col min="17" max="16384" width="8.85156" style="20" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="18" customWidth="1"/>
+    <col min="2" max="2" width="23.3516" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.85156" style="18" customWidth="1"/>
+    <col min="4" max="4" width="22" style="18" customWidth="1"/>
+    <col min="5" max="5" width="9.85156" style="18" customWidth="1"/>
+    <col min="6" max="16" width="8.85156" style="18" customWidth="1"/>
+    <col min="17" max="16384" width="8.85156" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="6">
+      <c r="A1" t="s" s="2">
         <v>68</v>
       </c>
       <c r="B1" t="s" s="2">
@@ -6411,22 +6404,22 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="21">
+      <c r="A2" s="19">
         <v>2007</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="20">
         <f>'Fixed Data'!B2/'China Debt Data'!$D29</f>
         <v>0.374961473430878</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="20">
         <f>'Fixed Data'!C2/'China Debt Data'!$D29</f>
         <v>0.400426473565856</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="20">
         <f>'Fixed Data'!D2/'China Debt Data'!$E29</f>
         <v>0.27042272250233</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="20">
         <f>'Fixed Data'!E2/'China Debt Data'!$E29</f>
         <v>0.281550095490674</v>
       </c>
@@ -6443,22 +6436,22 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="21">
+      <c r="A3" s="19">
         <v>2008</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="20">
         <f>'Fixed Data'!B3/'China Debt Data'!$D30</f>
         <v>0.343495015132398</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="20">
         <f>'Fixed Data'!C3/'China Debt Data'!$D30</f>
         <v>0.36456707212566</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="20">
         <f>'Fixed Data'!D3/'China Debt Data'!$E30</f>
         <v>0.285012373660398</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="20">
         <f>'Fixed Data'!E3/'China Debt Data'!$E30</f>
         <v>0.300506617695475</v>
       </c>
@@ -6475,22 +6468,22 @@
       <c r="P3" s="4"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="21">
+      <c r="A4" s="19">
         <v>2009</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="20">
         <f>'Fixed Data'!B4/'China Debt Data'!$D31</f>
         <v>0.392850914571945</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="20">
         <f>'Fixed Data'!C4/'China Debt Data'!$D31</f>
         <v>0.459990236418432</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="20">
         <f>'Fixed Data'!D4/'China Debt Data'!$E31</f>
         <v>0.325566075895756</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="20">
         <f>'Fixed Data'!E4/'China Debt Data'!$E31</f>
         <v>0.345658160755026</v>
       </c>
@@ -6507,22 +6500,22 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="21">
+      <c r="A5" s="19">
         <v>2010</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="20">
         <f>'Fixed Data'!B5/'China Debt Data'!$D32</f>
         <v>0.356923263061189</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="20">
         <f>'Fixed Data'!C5/'China Debt Data'!$D32</f>
         <v>0.42781037461118</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="20">
         <f>'Fixed Data'!D5/'China Debt Data'!$E32</f>
         <v>0.343979836792048</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="20">
         <f>'Fixed Data'!E5/'China Debt Data'!$E32</f>
         <v>0.373364289879477</v>
       </c>
@@ -6539,22 +6532,22 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="21">
+      <c r="A6" s="19">
         <v>2011</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <f>'Fixed Data'!B6/'China Debt Data'!$D33</f>
         <v>0.366489730326199</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="20">
         <f>'Fixed Data'!C6/'China Debt Data'!$D33</f>
         <v>0.439819270982273</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="20">
         <f>'Fixed Data'!D6/'China Debt Data'!$E33</f>
         <v>0.290835511721164</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="20">
         <f>'Fixed Data'!E6/'China Debt Data'!$E33</f>
         <v>0.314708006835005</v>
       </c>
@@ -6571,22 +6564,22 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="21">
+      <c r="A7" s="19">
         <v>2012</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <f>'Fixed Data'!B7/'China Debt Data'!$D34</f>
         <v>0.482603987076689</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="20">
         <f>'Fixed Data'!C7/'China Debt Data'!$D34</f>
         <v>0.5566333131703179</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="20">
         <f>'Fixed Data'!D7/'China Debt Data'!$E34</f>
         <v>0.268996814949373</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="20">
         <f>'Fixed Data'!E7/'China Debt Data'!$E34</f>
         <v>0.291065475273861</v>
       </c>
@@ -6603,22 +6596,22 @@
       <c r="P7" s="4"/>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="21">
+      <c r="A8" s="19">
         <v>2013</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <f>'Fixed Data'!B8/'China Debt Data'!$D35</f>
         <v>0.480385502400474</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="20">
         <f>'Fixed Data'!C8/'China Debt Data'!$D35</f>
         <v>0.554125517506092</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="20">
         <f>'Fixed Data'!D8/'China Debt Data'!$E35</f>
         <v>0.241582523059191</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="20">
         <f>'Fixed Data'!E8/'China Debt Data'!$E35</f>
         <v>0.262324230353552</v>
       </c>
@@ -6635,22 +6628,22 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="21">
+      <c r="A9" s="19">
         <v>2014</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <f>'Fixed Data'!B9/'China Debt Data'!$D36</f>
         <v>0.47855390524889</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="20">
         <f>'Fixed Data'!C9/'China Debt Data'!$D36</f>
         <v>0.573715434727406</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="20">
         <f>'Fixed Data'!D9/'China Debt Data'!$E36</f>
         <v>0.241707346748049</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="20">
         <f>'Fixed Data'!E9/'China Debt Data'!$E36</f>
         <v>0.294699918046763</v>
       </c>
@@ -6667,22 +6660,22 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="21">
+      <c r="A10" s="19">
         <v>2015</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <f>'Fixed Data'!B10/'China Debt Data'!$D37</f>
         <v>0.489994165679252</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="20">
         <f>'Fixed Data'!C10/'China Debt Data'!$D37</f>
         <v>0.57977685684475</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="20">
         <f>'Fixed Data'!D10/'China Debt Data'!$E37</f>
         <v>0.231469496165304</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="20">
         <f>'Fixed Data'!E10/'China Debt Data'!$E37</f>
         <v>0.287998082249146</v>
       </c>
@@ -6699,22 +6692,22 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="21">
+      <c r="A11" s="19">
         <v>2016</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <f>'Fixed Data'!B11/'China Debt Data'!$D38</f>
         <v>0.51482156386702</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="20">
         <f>'Fixed Data'!C11/'China Debt Data'!$D38</f>
         <v>0.603321723408874</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="20">
         <f>'Fixed Data'!D11/'China Debt Data'!$E38</f>
         <v>0.24193050877465</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="20">
         <f>'Fixed Data'!E11/'China Debt Data'!$E38</f>
         <v>0.331270869268697</v>
       </c>
@@ -6731,22 +6724,22 @@
       <c r="P11" s="4"/>
     </row>
     <row r="12" ht="15" customHeight="1">
-      <c r="A12" s="21">
+      <c r="A12" s="19">
         <v>2017</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="20">
         <f>'Fixed Data'!B12/'China Debt Data'!$D39</f>
         <v>0.523011502976599</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="20">
         <f>'Fixed Data'!C12/'China Debt Data'!$D39</f>
         <v>0.606651799388652</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="20">
         <f>'Fixed Data'!D12/'China Debt Data'!$E39</f>
         <v>0.264519935153729</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="20">
         <f>'Fixed Data'!E12/'China Debt Data'!$E39</f>
         <v>0.355133549987172</v>
       </c>
@@ -6763,7 +6756,7 @@
       <c r="P12" s="4"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="16"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -6781,7 +6774,7 @@
       <c r="P13" s="4"/>
     </row>
     <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="16"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -6799,7 +6792,7 @@
       <c r="P14" s="4"/>
     </row>
     <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="16"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -6833,23 +6826,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="23" customWidth="1"/>
-    <col min="2" max="2" width="23.3516" style="23" customWidth="1"/>
-    <col min="3" max="3" width="9.85156" style="23" customWidth="1"/>
-    <col min="4" max="4" width="22" style="23" customWidth="1"/>
-    <col min="5" max="5" width="9.85156" style="23" customWidth="1"/>
-    <col min="6" max="16" width="8.85156" style="23" customWidth="1"/>
-    <col min="17" max="16384" width="8.85156" style="23" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="21" customWidth="1"/>
+    <col min="2" max="2" width="23.3516" style="21" customWidth="1"/>
+    <col min="3" max="3" width="9.85156" style="21" customWidth="1"/>
+    <col min="4" max="4" width="22" style="21" customWidth="1"/>
+    <col min="5" max="5" width="9.85156" style="21" customWidth="1"/>
+    <col min="6" max="16" width="8.85156" style="21" customWidth="1"/>
+    <col min="17" max="16384" width="8.85156" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="6">
+      <c r="A1" t="s" s="2">
         <v>68</v>
       </c>
       <c r="B1" t="s" s="2">
@@ -6877,16 +6870,11 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="21">
-        <v>2000</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22">
-        <f>'Transposed'!B26/'China Debt Data'!D22</f>
-        <v>0.477510107191162</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20">
         <f>'Transposed'!D26/'China Debt Data'!E22</f>
         <v>0.415431766895427</v>
       </c>
@@ -6903,16 +6891,16 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="21">
-        <v>2001</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22">
-        <f>'Transposed'!B27/'China Debt Data'!D23</f>
-        <v>0.481038410967222</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22">
+      <c r="A3" s="19">
+        <v>1990</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20">
+        <f>'Transposed'!B16/'China Debt Data'!D12</f>
+        <v>0.619720016032953</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20">
         <f>'Transposed'!D27/'China Debt Data'!E23</f>
         <v>0.411212213114165</v>
       </c>
@@ -6929,16 +6917,16 @@
       <c r="P3" s="4"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="21">
-        <v>2002</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22">
-        <f>'Transposed'!B28/'China Debt Data'!D24</f>
-        <v>0.51687219983661</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22">
+      <c r="A4" s="19">
+        <v>1991</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20">
+        <f>'Transposed'!B17/'China Debt Data'!D13</f>
+        <v>0.634777680100318</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20">
         <f>'Transposed'!D28/'China Debt Data'!E24</f>
         <v>0.435826818121046</v>
       </c>
@@ -6955,16 +6943,16 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="21">
-        <v>2003</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22">
-        <f>'Transposed'!B29/'China Debt Data'!D25</f>
-        <v>0.496091464317099</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22">
+      <c r="A5" s="19">
+        <v>1992</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20">
+        <f>'Transposed'!B18/'China Debt Data'!D14</f>
+        <v>0.579464010182534</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20">
         <f>'Transposed'!D29/'China Debt Data'!E25</f>
         <v>0.408668201660593</v>
       </c>
@@ -6981,16 +6969,16 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="21">
-        <v>2004</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22">
-        <f>'Transposed'!B30/'China Debt Data'!D26</f>
-        <v>0.490400379995773</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22">
+      <c r="A6" s="19">
+        <v>1993</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20">
+        <f>'Transposed'!B19/'China Debt Data'!D15</f>
+        <v>0.577722582105792</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20">
         <f>'Transposed'!D30/'China Debt Data'!E26</f>
         <v>0.346191171838427</v>
       </c>
@@ -7007,16 +6995,16 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="21">
-        <v>2005</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22">
-        <f>'Transposed'!B31/'China Debt Data'!D27</f>
-        <v>0.404370521005547</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22">
+      <c r="A7" s="19">
+        <v>1994</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20">
+        <f>'Transposed'!B20/'China Debt Data'!D16</f>
+        <v>0.577651484623757</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20">
         <f>'Transposed'!D31/'China Debt Data'!E27</f>
         <v>0.289160669566428</v>
       </c>
@@ -7033,16 +7021,16 @@
       <c r="P7" s="4"/>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="21">
-        <v>2006</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22">
-        <f>'Transposed'!B32/'China Debt Data'!D28</f>
-        <v>0.36631073891035</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22">
+      <c r="A8" s="19">
+        <v>1995</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20">
+        <f>'Transposed'!B21/'China Debt Data'!D17</f>
+        <v>0.573659186668944</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20">
         <f>'Transposed'!D32/'China Debt Data'!E28</f>
         <v>0.272761412770624</v>
       </c>
@@ -7059,16 +7047,16 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="21">
-        <v>2007</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22">
-        <f>'Transposed'!B33/'China Debt Data'!D29</f>
-        <v>0.382294132969792</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22">
+      <c r="A9" s="19">
+        <v>1996</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20">
+        <f>'Transposed'!B22/'China Debt Data'!D18</f>
+        <v>0.517024674780388</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20">
         <f>'Transposed'!D33/'China Debt Data'!E29</f>
         <v>0.277668244361455</v>
       </c>
@@ -7085,16 +7073,16 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="21">
-        <v>2008</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22">
-        <f>'Transposed'!B34/'China Debt Data'!D30</f>
-        <v>0.350217198512939</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22">
+      <c r="A10" s="19">
+        <v>1997</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20">
+        <f>'Transposed'!B23/'China Debt Data'!D19</f>
+        <v>0.45317063799195</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20">
         <f>'Transposed'!D34/'China Debt Data'!E30</f>
         <v>0.291632580340995</v>
       </c>
@@ -7111,16 +7099,16 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="21">
-        <v>2009</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22">
-        <f>'Transposed'!B35/'China Debt Data'!D31</f>
-        <v>0.405383183921186</v>
-      </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22">
+      <c r="A11" s="19">
+        <v>1998</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20">
+        <f>'Transposed'!B24/'China Debt Data'!D20</f>
+        <v>0.491445108849702</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20">
         <f>'Transposed'!D35/'China Debt Data'!E31</f>
         <v>0.337530438637081</v>
       </c>
@@ -7137,16 +7125,16 @@
       <c r="P11" s="4"/>
     </row>
     <row r="12" ht="15" customHeight="1">
-      <c r="A12" s="21">
-        <v>2010</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22">
-        <f>'Transposed'!B36/'China Debt Data'!D32</f>
-        <v>0.382370140865808</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22">
+      <c r="A12" s="19">
+        <v>1999</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20">
+        <f>'Transposed'!B25/'China Debt Data'!D21</f>
+        <v>0.536534131502266</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20">
         <f>'Transposed'!D36/'China Debt Data'!E32</f>
         <v>0.356300005946401</v>
       </c>
@@ -7163,11 +7151,19 @@
       <c r="P12" s="4"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="16"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="19">
+        <v>2000</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20">
+        <f>'Transposed'!B26/'China Debt Data'!D22</f>
+        <v>0.477510107191162</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20">
+        <f>'Transposed'!D26/'China Debt Data'!E22</f>
+        <v>0.415431766895427</v>
+      </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -7181,16 +7177,18 @@
       <c r="P13" s="4"/>
     </row>
     <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="16"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="22">
-        <f>GEOMEAN(C2:C12)</f>
-        <v>0.428223188816735</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="22">
-        <f>GEOMEAN(E2:E12)</f>
-        <v>0.344420554300358</v>
+      <c r="A14" s="19">
+        <v>2001</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20">
+        <f>'Transposed'!B27/'China Debt Data'!D23</f>
+        <v>0.481038410967222</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20">
+        <f>'Transposed'!D27/'China Debt Data'!E23</f>
+        <v>0.411212213114165</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -7205,11 +7203,19 @@
       <c r="P14" s="4"/>
     </row>
     <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="16"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="A15" s="19">
+        <v>2002</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20">
+        <f>'Transposed'!B28/'China Debt Data'!D24</f>
+        <v>0.51687219983661</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20">
+        <f>'Transposed'!D28/'China Debt Data'!E24</f>
+        <v>0.435826818121046</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -7222,8 +7228,435 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" s="19">
+        <v>2003</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20">
+        <f>'Transposed'!B29/'China Debt Data'!D25</f>
+        <v>0.496091464317099</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20">
+        <f>'Transposed'!D29/'China Debt Data'!E25</f>
+        <v>0.408668201660593</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" s="19">
+        <v>2004</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20">
+        <f>'Transposed'!B30/'China Debt Data'!D26</f>
+        <v>0.490400379995773</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20">
+        <f>'Transposed'!D30/'China Debt Data'!E26</f>
+        <v>0.346191171838427</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" s="19">
+        <v>2005</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20">
+        <f>'Transposed'!B31/'China Debt Data'!D27</f>
+        <v>0.404370521005547</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20">
+        <f>'Transposed'!D31/'China Debt Data'!E27</f>
+        <v>0.289160669566428</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+    </row>
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" s="19">
+        <v>2006</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20">
+        <f>'Transposed'!B32/'China Debt Data'!D28</f>
+        <v>0.36631073891035</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20">
+        <f>'Transposed'!D32/'China Debt Data'!E28</f>
+        <v>0.272761412770624</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" ht="15" customHeight="1">
+      <c r="A20" s="19">
+        <v>2007</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20">
+        <f>'Transposed'!B33/'China Debt Data'!D29</f>
+        <v>0.382294132969792</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20">
+        <f>'Transposed'!D33/'China Debt Data'!E29</f>
+        <v>0.277668244361455</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" s="19">
+        <v>2008</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20">
+        <f>'Transposed'!B34/'China Debt Data'!D30</f>
+        <v>0.350217198512939</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20">
+        <f>'Transposed'!D34/'China Debt Data'!E30</f>
+        <v>0.291632580340995</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" ht="15" customHeight="1">
+      <c r="A22" s="19">
+        <v>2009</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20">
+        <f>'Transposed'!B35/'China Debt Data'!D31</f>
+        <v>0.405383183921186</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20">
+        <f>'Transposed'!D35/'China Debt Data'!E31</f>
+        <v>0.337530438637081</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+    </row>
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" s="19">
+        <v>2010</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20">
+        <f>'Transposed'!B36/'China Debt Data'!D32</f>
+        <v>0.382370140865808</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20">
+        <f>'Transposed'!D36/'China Debt Data'!E32</f>
+        <v>0.356300005946401</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="A24" s="19">
+        <v>2011</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20">
+        <f>'Transposed'!B37/'China Debt Data'!D33</f>
+        <v>0.395228519483047</v>
+      </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20">
+        <f>'Transposed'!D37/'China Debt Data'!E33</f>
+        <v>0.303118910239339</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" s="19">
+        <v>2012</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20">
+        <f>'Transposed'!B38/'China Debt Data'!D34</f>
+        <v>0.5223097175857579</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20">
+        <f>'Transposed'!D38/'China Debt Data'!E34</f>
+        <v>0.28375249667356</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" ht="15" customHeight="1">
+      <c r="A26" s="19">
+        <v>2013</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20">
+        <f>'Transposed'!B39/'China Debt Data'!D35</f>
+        <v>0.529297070619438</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20">
+        <f>'Transposed'!D39/'China Debt Data'!E35</f>
+        <v>0.259875186276587</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" ht="15" customHeight="1">
+      <c r="A27" s="19">
+        <v>2014</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20">
+        <f>'Transposed'!B40/'China Debt Data'!D36</f>
+        <v>0.532867177370385</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20">
+        <f>'Transposed'!D40/'China Debt Data'!E36</f>
+        <v>0.26273718205933</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" ht="15" customHeight="1">
+      <c r="A28" s="19">
+        <v>2015</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20">
+        <f>'Transposed'!B41/'China Debt Data'!D37</f>
+        <v>0.546254214434413</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20">
+        <f>'Transposed'!D41/'China Debt Data'!E37</f>
+        <v>0.253604380461716</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" s="19">
+        <v>2016</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20">
+        <f>'Transposed'!B42/'China Debt Data'!D38</f>
+        <v>0.572210269249258</v>
+      </c>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20">
+        <f>'Transposed'!D42/'China Debt Data'!E38</f>
+        <v>0.269337155441316</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" ht="15" customHeight="1">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="20">
+        <f>AVERAGE(C14:C21)</f>
+        <v>0.435949380814417</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="20">
+        <f>AVERAGE(E19:E26)</f>
+        <v>0.297829909405755</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" ht="15" customHeight="1">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="20">
+        <f>AVERAGE(C15:C20)</f>
+        <v>0.442723239505862</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A12">
+  <conditionalFormatting sqref="A1:A29">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
@@ -7244,9 +7677,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.8516" style="24" customWidth="1"/>
-    <col min="2" max="9" width="50.8516" style="24" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="24" customWidth="1"/>
+    <col min="1" max="1" width="15.8516" style="22" customWidth="1"/>
+    <col min="2" max="9" width="50.8516" style="22" customWidth="1"/>
+    <col min="10" max="16384" width="8.85156" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">

</xml_diff>